<commit_message>
conti camerino 2 dataframes su un foglio excell_01
</commit_message>
<xml_diff>
--- a/conti_camerino_modified_excel.xlsx
+++ b/conti_camerino_modified_excel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>gennaio</t>
   </si>
@@ -31,82 +31,136 @@
     <t>Voce</t>
   </si>
   <si>
-    <t>Entrate</t>
-  </si>
-  <si>
-    <t>Collette-Chiesa</t>
-  </si>
-  <si>
-    <t>Congrua</t>
-  </si>
-  <si>
-    <t>Interessi</t>
-  </si>
-  <si>
-    <t>Offerte</t>
-  </si>
-  <si>
-    <t>Pensioni</t>
-  </si>
-  <si>
-    <t>Salute</t>
-  </si>
-  <si>
-    <t>Servizi religiosi</t>
-  </si>
-  <si>
-    <t>Vendite varie</t>
-  </si>
-  <si>
-    <t>Cassette</t>
-  </si>
-  <si>
-    <t>Congrua fra Giacomo</t>
-  </si>
-  <si>
-    <t>Congrua fra Gianni</t>
-  </si>
-  <si>
-    <t>Offerta eccedenze Messa</t>
-  </si>
-  <si>
-    <t>Offerte libere</t>
-  </si>
-  <si>
-    <t>Presepio</t>
-  </si>
-  <si>
-    <t>Fr Tommaso Bellesi</t>
-  </si>
-  <si>
-    <t>Fr. Anastasio Artegiani</t>
-  </si>
-  <si>
-    <t>Fr. Giulio Criminesi</t>
-  </si>
-  <si>
-    <t>Fr. Mario Pigini</t>
-  </si>
-  <si>
-    <t>Medicine</t>
-  </si>
-  <si>
-    <t>Sanitaria</t>
-  </si>
-  <si>
-    <t>Loreto</t>
-  </si>
-  <si>
-    <t>Marmellata</t>
-  </si>
-  <si>
-    <t>Mercatino convento</t>
-  </si>
-  <si>
-    <t>Pasta</t>
-  </si>
-  <si>
-    <t>Vino</t>
+    <t>Uscite</t>
+  </si>
+  <si>
+    <t>Acquisti convento</t>
+  </si>
+  <si>
+    <t>Acquisti: Chiesa</t>
+  </si>
+  <si>
+    <t>Acquisti: Orto, Animali</t>
+  </si>
+  <si>
+    <t>Cultura</t>
+  </si>
+  <si>
+    <t>Elargizioni</t>
+  </si>
+  <si>
+    <t>Energia Elettrica</t>
+  </si>
+  <si>
+    <t>Ferie e Viaggi</t>
+  </si>
+  <si>
+    <t>Igiene</t>
+  </si>
+  <si>
+    <t>Imposte</t>
+  </si>
+  <si>
+    <t>Posta e cancelleria</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>Veicoli a motore</t>
+  </si>
+  <si>
+    <t>Vestiario</t>
+  </si>
+  <si>
+    <t>Vitto</t>
+  </si>
+  <si>
+    <t>Casalinghi</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>Materiale elettrico</t>
+  </si>
+  <si>
+    <t>Stampante_Fotocopiatrice</t>
+  </si>
+  <si>
+    <t>Ceri e Candele</t>
+  </si>
+  <si>
+    <t>Attrezzi agricoli manutenzione</t>
+  </si>
+  <si>
+    <t>Manutenzione api</t>
+  </si>
+  <si>
+    <t>Medicine animali - piante</t>
+  </si>
+  <si>
+    <t>Abbonamenti</t>
+  </si>
+  <si>
+    <t>Libri</t>
+  </si>
+  <si>
+    <t>Beneficenza 5%</t>
+  </si>
+  <si>
+    <t>ENEL</t>
+  </si>
+  <si>
+    <t>Carburante</t>
+  </si>
+  <si>
+    <t>Viaggi-Autostrada-Parcheggio</t>
+  </si>
+  <si>
+    <t>Detersivi</t>
+  </si>
+  <si>
+    <t>Igiene personale</t>
+  </si>
+  <si>
+    <t>Lavanderia</t>
+  </si>
+  <si>
+    <t>Imposte bancarie</t>
+  </si>
+  <si>
+    <t>Passaporto</t>
+  </si>
+  <si>
+    <t>Cancelleria</t>
+  </si>
+  <si>
+    <t>Scheda telefonica</t>
+  </si>
+  <si>
+    <t>Bollo Auto</t>
+  </si>
+  <si>
+    <t>Sandali - scarpe</t>
+  </si>
+  <si>
+    <t>Alimentari</t>
+  </si>
+  <si>
+    <t>Bartolazzi</t>
+  </si>
+  <si>
+    <t>Carne</t>
+  </si>
+  <si>
+    <t>Frutta e Verdura</t>
+  </si>
+  <si>
+    <t>Latte - Latticini</t>
+  </si>
+  <si>
+    <t>Pesce</t>
   </si>
 </sst>
 </file>
@@ -464,7 +518,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,65 +549,61 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>272</v>
+        <v>70.87</v>
       </c>
       <c r="E2">
-        <v>272</v>
+        <v>70.87</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D3">
-        <v>1060.05</v>
+        <v>38.56</v>
       </c>
       <c r="E3">
-        <v>1060.05</v>
+        <v>38.56</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D4">
-        <v>1028.81</v>
+        <v>20</v>
       </c>
       <c r="E4">
-        <v>1028.81</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D5">
-        <v>52.36</v>
+        <v>55.4</v>
       </c>
       <c r="E5">
-        <v>52.36</v>
+        <v>55.4</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -564,82 +614,86 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D7">
-        <v>394.29</v>
+        <v>274.33</v>
       </c>
       <c r="E7">
-        <v>394.29</v>
+        <v>274.33</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D8">
-        <v>128</v>
+        <v>630</v>
       </c>
       <c r="E8">
-        <v>128</v>
+        <v>630</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D9">
-        <v>635</v>
+        <v>75.18000000000001</v>
       </c>
       <c r="E9">
-        <v>635</v>
+        <v>75.18000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D10">
-        <v>635</v>
+        <v>100.32</v>
       </c>
       <c r="E10">
-        <v>635</v>
+        <v>100.32</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>635</v>
+        <v>30</v>
       </c>
       <c r="E11">
-        <v>635</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D12">
-        <v>635</v>
+        <v>130</v>
       </c>
       <c r="E12">
-        <v>635</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -648,132 +702,275 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D13">
-        <v>28.36</v>
+        <v>1185.57</v>
       </c>
       <c r="E13">
-        <v>28.36</v>
+        <v>1185.57</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D14">
-        <v>6.2</v>
+        <v>82.34999999999999</v>
       </c>
       <c r="E14">
-        <v>6.2</v>
+        <v>82.34999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D15">
-        <v>200</v>
+        <v>4.5</v>
       </c>
       <c r="E15">
-        <v>200</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C16" s="1" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D16">
-        <v>132.5</v>
+        <v>33.82</v>
       </c>
       <c r="E16">
-        <v>132.5</v>
+        <v>33.82</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D17">
-        <v>20</v>
+        <v>6.88</v>
       </c>
       <c r="E17">
-        <v>20</v>
+        <v>6.88</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D18">
-        <v>460</v>
+        <v>5.5</v>
       </c>
       <c r="E18">
-        <v>460</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C19" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D19">
-        <v>10</v>
+        <v>22.68</v>
       </c>
       <c r="E19">
-        <v>10</v>
+        <v>22.68</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D20">
-        <v>54.42</v>
+        <v>116</v>
       </c>
       <c r="E20">
-        <v>54.42</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21">
+        <v>35.98</v>
+      </c>
+      <c r="E21">
+        <v>35.98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23">
+        <v>121.78</v>
+      </c>
+      <c r="E23">
+        <v>121.78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24">
+        <v>24</v>
+      </c>
+      <c r="E24">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25">
+        <v>108.51</v>
+      </c>
+      <c r="E25">
+        <v>108.51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26">
+        <v>533</v>
+      </c>
+      <c r="E26">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27">
+        <v>86.09</v>
+      </c>
+      <c r="E27">
+        <v>86.09</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28">
+        <v>63.79</v>
+      </c>
+      <c r="E28">
+        <v>63.79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29">
+        <v>45.5</v>
+      </c>
+      <c r="E29">
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30">
+        <v>54.9</v>
+      </c>
+      <c r="E30">
+        <v>54.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21">
-        <v>228.77</v>
-      </c>
-      <c r="E21">
-        <v>228.77</v>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31">
+        <v>104.54</v>
+      </c>
+      <c r="E31">
+        <v>104.54</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A2:A20"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B20"/>
+  <mergeCells count="8">
+    <mergeCell ref="A2:A30"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B25:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>